<commit_message>
test du taux horraire
</commit_message>
<xml_diff>
--- a/app/static/excel/out.xlsx
+++ b/app/static/excel/out.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>RECAPITULATIF DES HEURES SUIVIES PAR STAGIARES EN M2 ISC _ 400 HEURES</t>
   </si>
@@ -116,10 +116,7 @@
     <t>Kitschminyof Stephan</t>
   </si>
   <si>
-    <t>Gallet Benjamin</t>
-  </si>
-  <si>
-    <t>Remarques :</t>
+    <t>G Benjamin</t>
   </si>
 </sst>
 </file>
@@ -143,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,6 +156,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE2EFDA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5D5FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDDFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -190,12 +199,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -567,22 +582,22 @@
       <c r="O6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="S6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="T6" t="s">
         <v>21</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="U6" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -608,119 +623,143 @@
         <v>6</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="S7" s="1"/>
-      <c r="U7" s="1"/>
+      <c r="S7" s="3"/>
+      <c r="U7" s="4"/>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="3">
+      <c r="A8" s="5">
         <v>1</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="3">
+      <c r="A9" s="5">
         <v>2</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="3">
+      <c r="A10" s="5">
         <v>3</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="3">
+      <c r="A11" s="5">
         <v>4</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="3">
+      <c r="A12" s="5">
         <v>5</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="3">
+      <c r="A13" s="5">
         <v>6</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="3">
+      <c r="A14" s="5">
         <v>7</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="3">
+      <c r="A15" s="5">
         <v>8</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="7" t="s">
         <v>25</v>
+      </c>
+      <c r="E15" s="7">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
manque diff CP & CA, total, barre en bas
</commit_message>
<xml_diff>
--- a/app/static/excel/out.xlsx
+++ b/app/static/excel/out.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>RECAPITULATIF DES HEURES SUIVIES PAR STAGIARES EN M2 ISC _ 400 HEURES</t>
   </si>
@@ -98,6 +98,9 @@
     <t>8 500,00€</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>Jacquet Virgile</t>
   </si>
   <si>
@@ -117,6 +120,9 @@
   </si>
   <si>
     <t>G Benjamin</t>
+  </si>
+  <si>
+    <t>FACTURATION trimestrielle heures suivies</t>
   </si>
 </sst>
 </file>
@@ -199,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -213,11 +219,17 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -594,7 +606,7 @@
       <c r="S6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="U6" s="4" t="s">
@@ -603,163 +615,533 @@
     </row>
     <row r="7" spans="1:21">
       <c r="D7" s="1"/>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="E7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" t="s">
+      <c r="K7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="O7" s="2"/>
+      <c r="P7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="S7" s="3"/>
+      <c r="T7" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="U7" s="4"/>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="5">
+      <c r="A8" s="9">
         <v>1</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
+        <f>E8+F8+G8+H8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <v>10</v>
+      </c>
+      <c r="M8" s="12">
+        <v>10</v>
+      </c>
+      <c r="N8" s="12">
+        <f>K8+L8+M8</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>0</v>
+      </c>
+      <c r="R8" s="13">
+        <v>0</v>
+      </c>
+      <c r="S8" s="13">
+        <f>P8+Q8+R8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="5">
+      <c r="A9" s="9">
         <v>2</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11">
+        <f>E9+F9+G9+H9</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="12">
+        <v>0</v>
+      </c>
+      <c r="L9" s="12">
+        <v>0</v>
+      </c>
+      <c r="M9" s="12">
+        <v>3</v>
+      </c>
+      <c r="N9" s="12">
+        <f>K9+L9+M9</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="P9" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="13">
+        <v>0</v>
+      </c>
+      <c r="R9" s="13">
+        <v>0</v>
+      </c>
+      <c r="S9" s="13">
+        <f>P9+Q9+R9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="9">
+        <v>3</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" s="5">
-        <v>3</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="E10" s="11">
+        <v>0</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
+        <f>E10+F10+G10+H10</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="12">
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <v>7</v>
+      </c>
+      <c r="N10" s="12">
+        <f>K10+L10+M10</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="13">
+        <v>0</v>
+      </c>
+      <c r="R10" s="13">
+        <v>0</v>
+      </c>
+      <c r="S10" s="13">
+        <f>P10+Q10+R10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="9">
+        <v>4</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" s="5">
-        <v>4</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="E11" s="11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="11">
+        <f>E11+F11+G11+H11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="11"/>
+      <c r="K11" s="12">
+        <v>0</v>
+      </c>
+      <c r="L11" s="12">
+        <v>0</v>
+      </c>
+      <c r="M11" s="12">
+        <v>0</v>
+      </c>
+      <c r="N11" s="12">
+        <f>K11+L11+M11</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="13">
+        <v>0</v>
+      </c>
+      <c r="R11" s="13">
+        <v>0</v>
+      </c>
+      <c r="S11" s="13">
+        <f>P11+Q11+R11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="9">
+        <v>5</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="5">
-        <v>5</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="E12" s="11">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+      <c r="I12" s="11">
+        <f>E12+F12+G12+H12</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
+        <v>7</v>
+      </c>
+      <c r="N12" s="12">
+        <f>K12+L12+M12</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P12" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="13">
+        <v>0</v>
+      </c>
+      <c r="R12" s="13">
+        <v>0</v>
+      </c>
+      <c r="S12" s="13">
+        <f>P12+Q12+R12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="9">
+        <v>6</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
-      <c r="A13" s="5">
-        <v>6</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="E13" s="11">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
+        <f>E13+F13+G13+H13</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="12">
+        <v>0</v>
+      </c>
+      <c r="L13" s="12">
+        <v>0</v>
+      </c>
+      <c r="M13" s="12">
+        <v>0</v>
+      </c>
+      <c r="N13" s="12">
+        <f>K13+L13+M13</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="13">
+        <v>0</v>
+      </c>
+      <c r="R13" s="13">
+        <v>0</v>
+      </c>
+      <c r="S13" s="13">
+        <f>P13+Q13+R13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="9">
+        <v>7</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
-      <c r="A14" s="5">
+      <c r="E14" s="11">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0</v>
+      </c>
+      <c r="H14" s="11">
+        <v>0</v>
+      </c>
+      <c r="I14" s="11">
+        <f>E14+F14+G14+H14</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12">
+        <v>0</v>
+      </c>
+      <c r="N14" s="12">
+        <f>K14+L14+M14</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P14" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="13">
+        <v>0</v>
+      </c>
+      <c r="R14" s="13">
+        <v>0</v>
+      </c>
+      <c r="S14" s="13">
+        <f>P14+Q14+R14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="9">
+        <v>8</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0</v>
+      </c>
+      <c r="I15" s="11">
+        <f>E15+F15+G15+H15</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="11"/>
+      <c r="K15" s="12">
+        <v>0</v>
+      </c>
+      <c r="L15" s="12">
+        <v>17</v>
+      </c>
+      <c r="M15" s="12">
         <v>7</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
-      <c r="A15" s="5">
-        <v>8</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="7">
+      <c r="N15" s="12">
+        <f>K15+L15+M15</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P15" s="13">
         <v>170</v>
+      </c>
+      <c r="Q15" s="13">
+        <v>68</v>
+      </c>
+      <c r="R15" s="13">
+        <v>170</v>
+      </c>
+      <c r="S15" s="13">
+        <f>P15+Q15+R15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
générateur fini (voir pour les CA)
</commit_message>
<xml_diff>
--- a/app/static/excel/out.xlsx
+++ b/app/static/excel/out.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
   <si>
     <t>RECAPITULATIF DES HEURES SUIVIES PAR STAGIARES EN M2 ISC _ 400 HEURES</t>
   </si>
@@ -98,9 +98,6 @@
     <t>8 500,00€</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Jacquet Virgile</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>G Benjamin</t>
+  </si>
+  <si>
+    <t>Totaux présence :</t>
   </si>
   <si>
     <t>FACTURATION trimestrielle heures suivies</t>
@@ -205,8 +205,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -223,13 +224,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,115 +557,116 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="Q6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="4" t="s">
+      <c r="T6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="U6" s="4" t="s">
+      <c r="U6" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="D7" s="1"/>
-      <c r="E7" s="5" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="6" t="s">
+      <c r="J7" s="2"/>
+      <c r="K7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="N7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="7" t="s">
+      <c r="O7" s="3"/>
+      <c r="P7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="Q7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="R7" s="7" t="s">
+      <c r="R7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="3"/>
-      <c r="T7" s="8" t="s">
+      <c r="S7" s="4"/>
+      <c r="T7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="U7" s="4"/>
+      <c r="U7" s="5"/>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="9">
+      <c r="A8" s="1">
         <v>1</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -684,7 +687,7 @@
       <c r="H8" s="11">
         <v>0</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="6">
         <f>E8+F8+G8+H8</f>
         <v>0</v>
       </c>
@@ -698,33 +701,36 @@
       <c r="M8" s="12">
         <v>10</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="7">
         <f>K8+L8+M8</f>
         <v>0</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="O8" s="12"/>
+      <c r="P8" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>0</v>
+      </c>
+      <c r="R8" s="13">
+        <v>0</v>
+      </c>
+      <c r="S8" s="13"/>
+      <c r="T8" s="9">
+        <f>I8+N8+P8</f>
+        <v>0</v>
+      </c>
+      <c r="U8" s="9">
+        <f>J8+O8+S8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="P8" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="13">
-        <v>0</v>
-      </c>
-      <c r="R8" s="13">
-        <v>0</v>
-      </c>
-      <c r="S8" s="13">
-        <f>P8+Q8+R8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="9">
-        <v>2</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>24</v>
@@ -744,7 +750,7 @@
       <c r="H9" s="11">
         <v>0</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="6">
         <f>E9+F9+G9+H9</f>
         <v>0</v>
       </c>
@@ -758,13 +764,11 @@
       <c r="M9" s="12">
         <v>3</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="7">
         <f>K9+L9+M9</f>
         <v>0</v>
       </c>
-      <c r="O9" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="O9" s="12"/>
       <c r="P9" s="13">
         <v>0</v>
       </c>
@@ -774,17 +778,22 @@
       <c r="R9" s="13">
         <v>0</v>
       </c>
-      <c r="S9" s="13">
-        <f>P9+Q9+R9</f>
+      <c r="S9" s="13"/>
+      <c r="T9" s="9">
+        <f>I9+N9+P9</f>
+        <v>0</v>
+      </c>
+      <c r="U9" s="9">
+        <f>J9+O9+S9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="9">
+      <c r="A10" s="1">
         <v>3</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>28</v>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>24</v>
@@ -804,7 +813,7 @@
       <c r="H10" s="11">
         <v>0</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="6">
         <f>E10+F10+G10+H10</f>
         <v>0</v>
       </c>
@@ -818,13 +827,11 @@
       <c r="M10" s="12">
         <v>7</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="7">
         <f>K10+L10+M10</f>
         <v>0</v>
       </c>
-      <c r="O10" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="O10" s="12"/>
       <c r="P10" s="13">
         <v>0</v>
       </c>
@@ -834,17 +841,22 @@
       <c r="R10" s="13">
         <v>0</v>
       </c>
-      <c r="S10" s="13">
-        <f>P10+Q10+R10</f>
+      <c r="S10" s="13"/>
+      <c r="T10" s="9">
+        <f>I10+N10+P10</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="9">
+        <f>J10+O10+S10</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="9">
+      <c r="A11" s="1">
         <v>4</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>29</v>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>24</v>
@@ -864,7 +876,7 @@
       <c r="H11" s="11">
         <v>0</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="6">
         <f>E11+F11+G11+H11</f>
         <v>0</v>
       </c>
@@ -878,13 +890,11 @@
       <c r="M11" s="12">
         <v>0</v>
       </c>
-      <c r="N11" s="12">
+      <c r="N11" s="7">
         <f>K11+L11+M11</f>
         <v>0</v>
       </c>
-      <c r="O11" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="O11" s="12"/>
       <c r="P11" s="13">
         <v>0</v>
       </c>
@@ -894,17 +904,22 @@
       <c r="R11" s="13">
         <v>0</v>
       </c>
-      <c r="S11" s="13">
-        <f>P11+Q11+R11</f>
+      <c r="S11" s="13"/>
+      <c r="T11" s="9">
+        <f>I11+N11+P11</f>
+        <v>0</v>
+      </c>
+      <c r="U11" s="9">
+        <f>J11+O11+S11</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="9">
+      <c r="A12" s="1">
         <v>5</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>30</v>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>24</v>
@@ -924,7 +939,7 @@
       <c r="H12" s="11">
         <v>0</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="6">
         <f>E12+F12+G12+H12</f>
         <v>0</v>
       </c>
@@ -938,13 +953,11 @@
       <c r="M12" s="12">
         <v>7</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="7">
         <f>K12+L12+M12</f>
         <v>0</v>
       </c>
-      <c r="O12" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="O12" s="12"/>
       <c r="P12" s="13">
         <v>0</v>
       </c>
@@ -954,17 +967,22 @@
       <c r="R12" s="13">
         <v>0</v>
       </c>
-      <c r="S12" s="13">
-        <f>P12+Q12+R12</f>
+      <c r="S12" s="13"/>
+      <c r="T12" s="9">
+        <f>I12+N12+P12</f>
+        <v>0</v>
+      </c>
+      <c r="U12" s="9">
+        <f>J12+O12+S12</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="9">
+      <c r="A13" s="1">
         <v>6</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>31</v>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>24</v>
@@ -984,7 +1002,7 @@
       <c r="H13" s="11">
         <v>0</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="6">
         <f>E13+F13+G13+H13</f>
         <v>0</v>
       </c>
@@ -998,13 +1016,11 @@
       <c r="M13" s="12">
         <v>0</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="7">
         <f>K13+L13+M13</f>
         <v>0</v>
       </c>
-      <c r="O13" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="O13" s="12"/>
       <c r="P13" s="13">
         <v>0</v>
       </c>
@@ -1014,17 +1030,22 @@
       <c r="R13" s="13">
         <v>0</v>
       </c>
-      <c r="S13" s="13">
-        <f>P13+Q13+R13</f>
+      <c r="S13" s="13"/>
+      <c r="T13" s="9">
+        <f>I13+N13+P13</f>
+        <v>0</v>
+      </c>
+      <c r="U13" s="9">
+        <f>J13+O13+S13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="9">
+      <c r="A14" s="1">
         <v>7</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>32</v>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>24</v>
@@ -1044,7 +1065,7 @@
       <c r="H14" s="11">
         <v>0</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="6">
         <f>E14+F14+G14+H14</f>
         <v>0</v>
       </c>
@@ -1058,13 +1079,11 @@
       <c r="M14" s="12">
         <v>0</v>
       </c>
-      <c r="N14" s="12">
+      <c r="N14" s="7">
         <f>K14+L14+M14</f>
         <v>0</v>
       </c>
-      <c r="O14" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="O14" s="12"/>
       <c r="P14" s="13">
         <v>0</v>
       </c>
@@ -1074,17 +1093,22 @@
       <c r="R14" s="13">
         <v>0</v>
       </c>
-      <c r="S14" s="13">
-        <f>P14+Q14+R14</f>
+      <c r="S14" s="13"/>
+      <c r="T14" s="9">
+        <f>I14+N14+P14</f>
+        <v>0</v>
+      </c>
+      <c r="U14" s="9">
+        <f>J14+O14+S14</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="9">
+      <c r="A15" s="1">
         <v>8</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>33</v>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>24</v>
@@ -1104,7 +1128,7 @@
       <c r="H15" s="11">
         <v>0</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="6">
         <f>E15+F15+G15+H15</f>
         <v>0</v>
       </c>
@@ -1118,13 +1142,11 @@
       <c r="M15" s="12">
         <v>7</v>
       </c>
-      <c r="N15" s="12">
+      <c r="N15" s="7">
         <f>K15+L15+M15</f>
         <v>0</v>
       </c>
-      <c r="O15" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="O15" s="12"/>
       <c r="P15" s="13">
         <v>170</v>
       </c>
@@ -1134,19 +1156,164 @@
       <c r="R15" s="13">
         <v>170</v>
       </c>
-      <c r="S15" s="13">
-        <f>P15+Q15+R15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
+      <c r="S15" s="13"/>
+      <c r="T15" s="9">
+        <f>I15+N15+P15</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="9">
+        <f>J15+O15+S15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="24" customHeight="1">
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11">
+        <f>SUM(E8:E15)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="11">
+        <f>SUM(F8:F15)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <f>SUM(G8:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="11">
+        <f>SUM(H8:H15)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="11">
+        <f>SUM(I8:I15)</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
+        <f>SUM(J8:J15)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="12">
+        <f>SUM(K8:K15)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
+        <f>SUM(L8:L15)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="12">
+        <f>SUM(M8:M15)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="12">
+        <f>SUM(N8:N15)</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="7">
+        <f>SUM(O8:O15)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="13">
+        <f>SUM(P8:P15)</f>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="13">
+        <f>SUM(Q8:Q15)</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="13">
+        <f>SUM(R8:R15)</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="8">
+        <f>SUM(S8:S15)</f>
+        <v>0</v>
+      </c>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+    </row>
+    <row r="17" spans="2:21" ht="24" customHeight="1">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="6">
+        <f> </f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="7">
+        <f> </f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="8">
+        <f> </f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="9">
+        <f> </f>
+        <v>0</v>
+      </c>
+      <c r="U17" s="9">
+        <f> </f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21">
+      <c r="B18" s="15" t="s">
         <v>34</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="6">
+        <f>SUM(J8:J15)</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="7">
+        <f>SUM(O8:O15)</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="8">
+        <f>SUM(S8:S15)</f>
+        <v>0</v>
+      </c>
+      <c r="T18" s="9">
+        <f>SUM(T8:T15)</f>
+        <v>0</v>
+      </c>
+      <c r="U18" s="9">
+        <f>SUM(U8:U15)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>

</xml_diff>